<commit_message>
More item data updates - Modified the first iteration script to auto-plant farms in slots 1-4
</commit_message>
<xml_diff>
--- a/data/content/items.xlsx
+++ b/data/content/items.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dev\GHO\data\content\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_dev\SMC\GHO-master\data\content\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="274">
   <si>
     <t>id</t>
   </si>
@@ -747,13 +747,112 @@
   </si>
   <si>
     <t>images/oil-status-bar.png</t>
+  </si>
+  <si>
+    <t>dottedGreenLeafSeed</t>
+  </si>
+  <si>
+    <t>greenLeafSeed</t>
+  </si>
+  <si>
+    <t>limeLeafSeed</t>
+  </si>
+  <si>
+    <t>crystalLeafSeed</t>
+  </si>
+  <si>
+    <t>redMushroomSeed</t>
+  </si>
+  <si>
+    <t>goldLeafSead</t>
+  </si>
+  <si>
+    <t>blueMushroomSeed</t>
+  </si>
+  <si>
+    <t>Dotted Green Leaf Seed</t>
+  </si>
+  <si>
+    <t>Green Leaf Seed</t>
+  </si>
+  <si>
+    <t>Lime Leaf Seed</t>
+  </si>
+  <si>
+    <t>Crystal Leaf Seed</t>
+  </si>
+  <si>
+    <t>Red Mushroom Seed</t>
+  </si>
+  <si>
+    <t>Blue Mushroom Seed</t>
+  </si>
+  <si>
+    <t>Gold Leaf Seed</t>
+  </si>
+  <si>
+    <t>brewingBook</t>
+  </si>
+  <si>
+    <t>Brewing Book</t>
+  </si>
+  <si>
+    <t>anvil</t>
+  </si>
+  <si>
+    <t>Anvil</t>
+  </si>
+  <si>
+    <t>1000|2000|5000|7500|10000|13000|19000|28000|35000|50000</t>
+  </si>
+  <si>
+    <t>100|200|500|750|1000|1300|1900|2800|3500|5000</t>
+  </si>
+  <si>
+    <t>legacyId</t>
+  </si>
+  <si>
+    <t>xpGain</t>
+  </si>
+  <si>
+    <t>dottedGreenLeaf:5</t>
+  </si>
+  <si>
+    <t>redMushroom:50</t>
+  </si>
+  <si>
+    <t>greenLeaf:1</t>
+  </si>
+  <si>
+    <t>redMushroom:150</t>
+  </si>
+  <si>
+    <t>dottedGreenLeaf:10</t>
+  </si>
+  <si>
+    <t>bronzeBar:1</t>
+  </si>
+  <si>
+    <t>ironBar:1</t>
+  </si>
+  <si>
+    <t>silverBar:1</t>
+  </si>
+  <si>
+    <t>limeLeaf:5</t>
+  </si>
+  <si>
+    <t>blueMushroom:25</t>
+  </si>
+  <si>
+    <t>blewitMushroom</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -781,6 +880,12 @@
       <name val="Courier New"/>
       <family val="3"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial Unicode MS"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -802,7 +907,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -811,6 +916,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1093,1400 +1201,1737 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T75"/>
+  <dimension ref="A1:V77"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N11" sqref="N11"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="34.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="35.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="35.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="16.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>261</v>
       </c>
       <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
+        <v>262</v>
+      </c>
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>168</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>166</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>167</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>9</v>
       </c>
-      <c r="N1" t="s">
+      <c r="P1" t="s">
         <v>10</v>
       </c>
-      <c r="O1" t="s">
+      <c r="Q1" t="s">
         <v>114</v>
       </c>
-      <c r="P1" t="s">
+      <c r="R1" t="s">
         <v>115</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="S1" t="s">
         <v>116</v>
       </c>
-      <c r="R1" t="s">
+      <c r="T1" t="s">
         <v>117</v>
       </c>
-      <c r="S1" t="s">
+      <c r="U1" t="s">
         <v>118</v>
       </c>
-      <c r="T1" t="s">
+      <c r="V1" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>12</v>
       </c>
-      <c r="F2" t="b">
-        <v>1</v>
-      </c>
-      <c r="G2">
+      <c r="H2" t="b">
+        <v>1</v>
+      </c>
+      <c r="I2">
         <v>25</v>
       </c>
-      <c r="H2" t="b">
-        <v>1</v>
-      </c>
-      <c r="M2" s="1" t="s">
+      <c r="J2" t="b">
+        <v>1</v>
+      </c>
+      <c r="O2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="P2" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="1"/>
+      <c r="C3" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="D3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E3">
+      <c r="E3" s="1"/>
+      <c r="F3" t="b">
+        <v>1</v>
+      </c>
+      <c r="G3">
         <v>500000</v>
       </c>
-      <c r="H3" t="b">
-        <v>1</v>
-      </c>
-      <c r="M3" s="1" t="s">
+      <c r="J3" t="b">
+        <v>1</v>
+      </c>
+      <c r="O3" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="N3" s="1" t="s">
+      <c r="P3" s="1" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="1"/>
+      <c r="C4" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="D4" t="b">
-        <v>1</v>
-      </c>
-      <c r="E4" s="3">
+      <c r="E4" s="1"/>
+      <c r="F4" t="b">
+        <v>1</v>
+      </c>
+      <c r="G4" s="3">
         <v>2000000</v>
       </c>
-      <c r="H4" t="b">
-        <v>1</v>
-      </c>
-      <c r="M4" s="1" t="s">
+      <c r="J4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O4" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="N4" s="1" t="s">
+      <c r="P4" s="1" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="1"/>
+      <c r="C5" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="D5" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="D5" t="b">
-        <v>1</v>
-      </c>
-      <c r="E5" s="3">
+      <c r="E5" s="1"/>
+      <c r="F5" t="b">
+        <v>1</v>
+      </c>
+      <c r="G5" s="3">
         <v>17500000</v>
       </c>
-      <c r="H5" t="b">
-        <v>1</v>
-      </c>
-      <c r="M5" s="1" t="s">
+      <c r="J5" t="b">
+        <v>1</v>
+      </c>
+      <c r="O5" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="N5" s="1" t="s">
+      <c r="P5" s="1" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="M6" s="1" t="s">
+      <c r="B6" s="1"/>
+      <c r="O6" s="1" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="1"/>
+      <c r="C7" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>93</v>
       </c>
-      <c r="M7" s="1" t="s">
+      <c r="O7" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="N7" t="s">
+      <c r="P7" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="1"/>
+      <c r="C8" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>94</v>
       </c>
-      <c r="M8" s="1" t="s">
+      <c r="O8" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="N8" t="s">
+      <c r="P8" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="1"/>
+      <c r="C9" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>95</v>
       </c>
-      <c r="M9" s="1" t="s">
+      <c r="O9" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="N9" t="s">
+      <c r="P9" t="s">
         <v>92</v>
       </c>
-      <c r="O9" t="s">
+      <c r="Q9" t="s">
         <v>120</v>
       </c>
-      <c r="P9" t="s">
+      <c r="R9" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="2"/>
+      <c r="C10" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="H10" t="b">
-        <v>1</v>
-      </c>
-      <c r="M10" s="1" t="s">
+      <c r="J10" t="b">
+        <v>1</v>
+      </c>
+      <c r="O10" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="N10" t="s">
+      <c r="P10" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="2"/>
+      <c r="C11" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="H11" t="b">
-        <v>1</v>
-      </c>
-      <c r="M11" s="1" t="s">
+      <c r="I11">
+        <v>10</v>
+      </c>
+      <c r="J11" t="b">
+        <v>1</v>
+      </c>
+      <c r="O11" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="N11" t="s">
+      <c r="P11" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="2"/>
+      <c r="C12" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="H12" t="b">
-        <v>1</v>
-      </c>
-      <c r="M12" s="1" t="s">
+      <c r="I12">
+        <v>20</v>
+      </c>
+      <c r="J12" t="b">
+        <v>1</v>
+      </c>
+      <c r="O12" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="N12" t="s">
+      <c r="P12" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="2"/>
+      <c r="C13" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="H13" t="b">
-        <v>1</v>
-      </c>
-      <c r="M13" s="1" t="s">
+      <c r="I13">
+        <v>2</v>
+      </c>
+      <c r="J13" t="b">
+        <v>1</v>
+      </c>
+      <c r="O13" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="N13" t="s">
+      <c r="P13" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="2"/>
+      <c r="C14" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="H14" t="b">
-        <v>1</v>
-      </c>
-      <c r="M14" s="1" t="s">
+      <c r="E14" s="4">
+        <v>1E-3</v>
+      </c>
+      <c r="I14">
+        <v>1</v>
+      </c>
+      <c r="J14" t="b">
+        <v>1</v>
+      </c>
+      <c r="O14" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="N14" t="s">
+      <c r="P14" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" s="2"/>
+      <c r="C15" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="H15" t="b">
-        <v>1</v>
-      </c>
-      <c r="M15" s="1" t="s">
+      <c r="E15" s="4">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="I15">
+        <v>5</v>
+      </c>
+      <c r="J15" t="b">
+        <v>1</v>
+      </c>
+      <c r="O15" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="N15" t="s">
+      <c r="P15" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" s="2"/>
+      <c r="C16" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="H16" t="b">
-        <v>1</v>
-      </c>
-      <c r="M16" s="1" t="s">
+      <c r="E16" s="4">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="I16">
+        <v>5</v>
+      </c>
+      <c r="J16" t="b">
+        <v>1</v>
+      </c>
+      <c r="O16" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="N16" t="s">
+      <c r="P16" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" s="2"/>
+      <c r="C17" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="H17" t="b">
-        <v>1</v>
-      </c>
-      <c r="M17" s="1" t="s">
+      <c r="E17" s="4">
+        <v>0.03</v>
+      </c>
+      <c r="I17">
+        <v>20</v>
+      </c>
+      <c r="J17" t="b">
+        <v>1</v>
+      </c>
+      <c r="O17" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="N17" t="s">
+      <c r="P17" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" s="2"/>
+      <c r="C18" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="H18" t="b">
-        <v>1</v>
-      </c>
-      <c r="M18" s="1" t="s">
+      <c r="E18" s="4">
+        <v>0.08</v>
+      </c>
+      <c r="I18">
+        <v>50</v>
+      </c>
+      <c r="J18" t="b">
+        <v>1</v>
+      </c>
+      <c r="O18" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="N18" t="s">
+      <c r="P18" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" s="2"/>
+      <c r="C19" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="H19" t="b">
-        <v>1</v>
-      </c>
-      <c r="M19" s="1" t="s">
+      <c r="E19" s="4">
+        <v>0.12</v>
+      </c>
+      <c r="I19">
+        <v>100</v>
+      </c>
+      <c r="J19" t="b">
+        <v>1</v>
+      </c>
+      <c r="O19" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="N19" t="s">
+      <c r="P19" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" s="2"/>
+      <c r="C20" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="H20" t="b">
-        <v>1</v>
-      </c>
-      <c r="M20" s="1" t="s">
+      <c r="E20" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="I20">
+        <v>130</v>
+      </c>
+      <c r="J20" t="b">
+        <v>1</v>
+      </c>
+      <c r="O20" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="N20" t="s">
+      <c r="P20" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B21" s="2"/>
+      <c r="C21" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="H21" t="b">
-        <v>1</v>
-      </c>
-      <c r="M21" s="1" t="s">
+      <c r="E21" s="4">
+        <v>1</v>
+      </c>
+      <c r="I21">
+        <v>185</v>
+      </c>
+      <c r="J21" t="b">
+        <v>1</v>
+      </c>
+      <c r="O21" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="N21" t="s">
+      <c r="P21" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B22" s="2"/>
+      <c r="C22" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="H22" t="b">
-        <v>1</v>
-      </c>
-      <c r="M22" s="1" t="s">
+      <c r="E22" s="4">
+        <v>2</v>
+      </c>
+      <c r="J22" t="b">
+        <v>1</v>
+      </c>
+      <c r="O22" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="N22" t="s">
+      <c r="P22" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B23" s="2"/>
+      <c r="C23" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="H23" t="b">
-        <v>1</v>
-      </c>
-      <c r="M23" s="1" t="s">
+      <c r="E23" s="4">
+        <v>3.5</v>
+      </c>
+      <c r="J23" t="b">
+        <v>1</v>
+      </c>
+      <c r="O23" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="N23" t="s">
+      <c r="P23" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B24" s="2"/>
+      <c r="C24" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="H24" t="b">
-        <v>1</v>
-      </c>
-      <c r="M24" s="1" t="s">
+      <c r="I24">
+        <v>100000</v>
+      </c>
+      <c r="J24" t="b">
+        <v>1</v>
+      </c>
+      <c r="O24" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="N24" t="s">
+      <c r="P24" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="B25" s="2"/>
+      <c r="C25" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="H25" t="b">
-        <v>1</v>
-      </c>
-      <c r="M25" s="1" t="s">
+      <c r="I25">
+        <v>200000</v>
+      </c>
+      <c r="J25" t="b">
+        <v>1</v>
+      </c>
+      <c r="O25" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="N25" t="s">
+      <c r="P25" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B26" s="2"/>
+      <c r="C26" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="H26" t="b">
-        <v>1</v>
-      </c>
-      <c r="M26" s="1" t="s">
+      <c r="I26">
+        <v>300000</v>
+      </c>
+      <c r="J26" t="b">
+        <v>1</v>
+      </c>
+      <c r="O26" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="N26" t="s">
+      <c r="P26" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="B27" s="2"/>
+      <c r="C27" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="H27" t="b">
-        <v>1</v>
-      </c>
-      <c r="M27" s="1" t="s">
+      <c r="I27">
+        <v>1000000</v>
+      </c>
+      <c r="J27" t="b">
+        <v>1</v>
+      </c>
+      <c r="O27" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="N27" t="s">
+      <c r="P27" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B28" s="2"/>
+      <c r="C28" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="H28" t="b">
-        <v>1</v>
-      </c>
-      <c r="M28" s="1" t="s">
+      <c r="J28" t="b">
+        <v>1</v>
+      </c>
+      <c r="O28" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="N28" t="s">
+      <c r="P28" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B29" s="2"/>
+      <c r="C29" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="H29" t="b">
-        <v>1</v>
-      </c>
-      <c r="M29" s="1" t="s">
+      <c r="J29" t="b">
+        <v>1</v>
+      </c>
+      <c r="O29" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="N29" t="s">
+      <c r="P29" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="B30" s="2"/>
+      <c r="C30" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="H30" t="b">
-        <v>1</v>
-      </c>
-      <c r="M30" s="1" t="s">
+      <c r="I30">
+        <v>15</v>
+      </c>
+      <c r="J30" t="b">
+        <v>1</v>
+      </c>
+      <c r="O30" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="N30" t="s">
+      <c r="P30" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="B31" s="2"/>
+      <c r="C31" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="H31" t="b">
-        <v>1</v>
-      </c>
-      <c r="M31" s="1" t="s">
+      <c r="I31">
+        <v>35</v>
+      </c>
+      <c r="J31" t="b">
+        <v>1</v>
+      </c>
+      <c r="O31" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="N31" t="s">
+      <c r="P31" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="B32" s="2"/>
+      <c r="C32" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="H32" t="b">
-        <v>1</v>
-      </c>
-      <c r="M32" s="1" t="s">
+      <c r="I32">
+        <v>75</v>
+      </c>
+      <c r="J32" t="b">
+        <v>1</v>
+      </c>
+      <c r="O32" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="N32" t="s">
+      <c r="P32" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="B33" s="2"/>
+      <c r="C33" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="H33" t="b">
-        <v>1</v>
-      </c>
-      <c r="M33" s="1" t="s">
+      <c r="I33">
+        <v>250</v>
+      </c>
+      <c r="J33" t="b">
+        <v>1</v>
+      </c>
+      <c r="O33" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="N33" t="s">
+      <c r="P33" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="B34" s="2"/>
+      <c r="C34" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="H34" t="b">
-        <v>1</v>
-      </c>
-      <c r="M34" s="1" t="s">
+      <c r="I34">
+        <v>500</v>
+      </c>
+      <c r="J34" t="b">
+        <v>1</v>
+      </c>
+      <c r="O34" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="N34" t="s">
+      <c r="P34" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="B35" s="2"/>
+      <c r="C35" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="H35" t="b">
-        <v>1</v>
-      </c>
-      <c r="M35" s="1" t="s">
+      <c r="I35">
+        <v>20</v>
+      </c>
+      <c r="J35" t="b">
+        <v>1</v>
+      </c>
+      <c r="O35" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="N35" t="s">
+      <c r="P35" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B36" s="1" t="s">
+      <c r="B36" s="2"/>
+      <c r="C36" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="H36" t="b">
-        <v>1</v>
-      </c>
-      <c r="M36" s="1" t="s">
+      <c r="I36">
+        <v>100</v>
+      </c>
+      <c r="J36" t="b">
+        <v>1</v>
+      </c>
+      <c r="O36" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="N36" t="s">
+      <c r="P36" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B37" s="1" t="s">
+      <c r="B37" s="2"/>
+      <c r="C37" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="H37" t="b">
-        <v>1</v>
-      </c>
-      <c r="M37" s="1" t="s">
+      <c r="I37">
+        <v>500</v>
+      </c>
+      <c r="J37" t="b">
+        <v>1</v>
+      </c>
+      <c r="O37" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="N37" t="s">
+      <c r="P37" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B38" s="1" t="s">
+      <c r="B38" s="2"/>
+      <c r="C38" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="H38" t="b">
-        <v>1</v>
-      </c>
-      <c r="M38" s="1" t="s">
+      <c r="I38">
+        <v>1000</v>
+      </c>
+      <c r="J38" t="b">
+        <v>1</v>
+      </c>
+      <c r="O38" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="N38" t="s">
+      <c r="P38" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B39" s="1" t="s">
+      <c r="B39" s="2"/>
+      <c r="C39" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="H39" t="b">
-        <v>1</v>
-      </c>
-      <c r="M39" s="1" t="s">
+      <c r="I39">
+        <v>5000</v>
+      </c>
+      <c r="J39" t="b">
+        <v>1</v>
+      </c>
+      <c r="O39" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="N39" t="s">
+      <c r="P39" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="B40" s="1" t="s">
+      <c r="B40" s="2"/>
+      <c r="C40" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="H40" t="b">
-        <v>1</v>
-      </c>
-      <c r="M40" s="1" t="s">
+      <c r="I40">
+        <v>100</v>
+      </c>
+      <c r="J40" t="b">
+        <v>1</v>
+      </c>
+      <c r="O40" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="N40" t="s">
+      <c r="P40" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="B41" s="1" t="s">
+      <c r="B41" s="4" t="s">
+        <v>273</v>
+      </c>
+      <c r="C41" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="H41" t="b">
-        <v>1</v>
-      </c>
-      <c r="M41" s="1" t="s">
+      <c r="I41">
+        <v>250</v>
+      </c>
+      <c r="J41" t="b">
+        <v>1</v>
+      </c>
+      <c r="O41" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="N41" t="s">
+      <c r="P41" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="B42" s="1" t="s">
+      <c r="B42" s="4"/>
+      <c r="C42" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="H42" t="b">
-        <v>1</v>
-      </c>
-      <c r="M42" s="1" t="s">
+      <c r="J42" t="b">
+        <v>1</v>
+      </c>
+      <c r="O42" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="N42" t="s">
+      <c r="P42" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="Q42" s="4" t="s">
+        <v>263</v>
+      </c>
+      <c r="R42" s="2" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="43" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="B43" s="1" t="s">
+      <c r="B43" s="4"/>
+      <c r="C43" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="H43" t="b">
-        <v>1</v>
-      </c>
-      <c r="M43" s="1" t="s">
+      <c r="J43" t="b">
+        <v>1</v>
+      </c>
+      <c r="O43" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="N43" t="s">
+      <c r="P43" t="s">
         <v>228</v>
       </c>
-    </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="Q43" s="4" t="s">
+        <v>263</v>
+      </c>
+      <c r="R43" s="4" t="s">
+        <v>265</v>
+      </c>
+      <c r="S43" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="44" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="B44" s="1" t="s">
+      <c r="B44" s="4"/>
+      <c r="C44" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="H44" t="b">
-        <v>1</v>
-      </c>
-      <c r="M44" s="1" t="s">
+      <c r="J44" t="b">
+        <v>1</v>
+      </c>
+      <c r="O44" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="N44" t="s">
+      <c r="P44" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="Q44" s="4" t="s">
+        <v>267</v>
+      </c>
+      <c r="R44" t="s">
+        <v>268</v>
+      </c>
+      <c r="S44" t="s">
+        <v>269</v>
+      </c>
+      <c r="T44" t="s">
+        <v>121</v>
+      </c>
+      <c r="U44" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="45" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="B45" s="1" t="s">
+      <c r="B45" s="4"/>
+      <c r="C45" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="H45" t="b">
-        <v>1</v>
-      </c>
-      <c r="M45" s="1" t="s">
+      <c r="J45" t="b">
+        <v>1</v>
+      </c>
+      <c r="O45" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="N45" t="s">
+      <c r="P45" t="s">
         <v>230</v>
       </c>
-    </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="Q45" s="4" t="s">
+        <v>271</v>
+      </c>
+      <c r="R45" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="S45" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="46" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="B46" s="1" t="s">
+      <c r="B46" s="2"/>
+      <c r="C46" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="H46" t="b">
-        <v>1</v>
-      </c>
-      <c r="K46" t="b">
-        <v>1</v>
-      </c>
-      <c r="L46">
-        <v>1</v>
-      </c>
-      <c r="M46" s="1" t="s">
+      <c r="J46" t="b">
+        <v>1</v>
+      </c>
+      <c r="M46" t="b">
+        <v>1</v>
+      </c>
+      <c r="N46">
+        <v>1</v>
+      </c>
+      <c r="O46" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="N46" t="s">
+      <c r="P46" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="B47" s="1" t="s">
+      <c r="B47" s="2"/>
+      <c r="C47" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="H47" t="b">
-        <v>1</v>
-      </c>
-      <c r="K47" t="b">
-        <v>1</v>
-      </c>
-      <c r="L47">
-        <v>1</v>
-      </c>
-      <c r="M47" s="1" t="s">
+      <c r="J47" t="b">
+        <v>1</v>
+      </c>
+      <c r="M47" t="b">
+        <v>1</v>
+      </c>
+      <c r="N47">
+        <v>1</v>
+      </c>
+      <c r="O47" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="N47" t="s">
+      <c r="P47" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="B48" s="1" t="s">
+      <c r="B48" s="2"/>
+      <c r="C48" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="H48" t="b">
-        <v>1</v>
-      </c>
-      <c r="K48" t="b">
-        <v>1</v>
-      </c>
-      <c r="L48">
-        <v>1</v>
-      </c>
-      <c r="M48" s="1" t="s">
+      <c r="J48" t="b">
+        <v>1</v>
+      </c>
+      <c r="M48" t="b">
+        <v>1</v>
+      </c>
+      <c r="N48">
+        <v>1</v>
+      </c>
+      <c r="O48" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="N48" t="s">
+      <c r="P48" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="B49" s="1" t="s">
+      <c r="B49" s="2"/>
+      <c r="C49" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="H49" t="b">
-        <v>1</v>
-      </c>
-      <c r="K49" t="b">
-        <v>1</v>
-      </c>
-      <c r="L49">
-        <v>1</v>
-      </c>
-      <c r="M49" s="1" t="s">
+      <c r="J49" t="b">
+        <v>1</v>
+      </c>
+      <c r="M49" t="b">
+        <v>1</v>
+      </c>
+      <c r="N49">
+        <v>1</v>
+      </c>
+      <c r="O49" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="N49" t="s">
+      <c r="P49" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="B50" s="1" t="s">
+      <c r="B50" s="2"/>
+      <c r="C50" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="H50" t="b">
-        <v>1</v>
-      </c>
-      <c r="K50" t="b">
-        <v>1</v>
-      </c>
-      <c r="L50">
-        <v>1</v>
-      </c>
-      <c r="M50" s="1" t="s">
+      <c r="J50" t="b">
+        <v>1</v>
+      </c>
+      <c r="M50" t="b">
+        <v>1</v>
+      </c>
+      <c r="N50">
+        <v>1</v>
+      </c>
+      <c r="O50" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="N50" t="s">
+      <c r="P50" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="B51" s="1" t="s">
+      <c r="B51" s="2"/>
+      <c r="C51" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="H51" t="b">
-        <v>1</v>
-      </c>
-      <c r="K51" t="b">
-        <v>1</v>
-      </c>
-      <c r="L51">
-        <v>1</v>
-      </c>
-      <c r="M51" s="1" t="s">
+      <c r="J51" t="b">
+        <v>1</v>
+      </c>
+      <c r="M51" t="b">
+        <v>1</v>
+      </c>
+      <c r="N51">
+        <v>1</v>
+      </c>
+      <c r="O51" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="N51" t="s">
+      <c r="P51" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="B52" s="1" t="s">
+      <c r="B52" s="2"/>
+      <c r="C52" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="H52" t="b">
-        <v>1</v>
-      </c>
-      <c r="K52" t="b">
-        <v>1</v>
-      </c>
-      <c r="L52">
-        <v>1</v>
-      </c>
-      <c r="M52" s="1" t="s">
+      <c r="J52" t="b">
+        <v>1</v>
+      </c>
+      <c r="M52" t="b">
+        <v>1</v>
+      </c>
+      <c r="N52">
+        <v>1</v>
+      </c>
+      <c r="O52" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="N52" t="s">
+      <c r="P52" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="B53" s="1" t="s">
+      <c r="B53" s="2"/>
+      <c r="C53" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="H53" t="b">
-        <v>1</v>
-      </c>
-      <c r="K53" t="b">
-        <v>1</v>
-      </c>
-      <c r="L53">
+      <c r="J53" t="b">
+        <v>1</v>
+      </c>
+      <c r="M53" t="b">
+        <v>1</v>
+      </c>
+      <c r="N53">
         <v>10</v>
       </c>
-      <c r="M53" s="1" t="s">
+      <c r="O53" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="N53" t="s">
+      <c r="P53" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="B54" s="1" t="s">
+      <c r="B54" s="2"/>
+      <c r="C54" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="H54" t="b">
-        <v>1</v>
-      </c>
-      <c r="K54" t="b">
-        <v>1</v>
-      </c>
-      <c r="L54">
+      <c r="J54" t="b">
+        <v>1</v>
+      </c>
+      <c r="M54" t="b">
+        <v>1</v>
+      </c>
+      <c r="N54">
         <v>10</v>
       </c>
-      <c r="M54" s="1" t="s">
+      <c r="O54" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="N54" t="s">
+      <c r="P54" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="B55" s="1" t="s">
+      <c r="B55" s="2"/>
+      <c r="C55" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="H55" t="b">
-        <v>1</v>
-      </c>
-      <c r="K55" t="b">
-        <v>1</v>
-      </c>
-      <c r="L55">
+      <c r="J55" t="b">
+        <v>1</v>
+      </c>
+      <c r="M55" t="b">
+        <v>1</v>
+      </c>
+      <c r="N55">
         <v>10</v>
       </c>
-      <c r="M55" s="1" t="s">
+      <c r="O55" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="N55" t="s">
+      <c r="P55" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="B56" s="1" t="s">
+      <c r="B56" s="2"/>
+      <c r="C56" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="H56" t="b">
-        <v>1</v>
-      </c>
-      <c r="M56" s="1" t="s">
+      <c r="J56" t="b">
+        <v>1</v>
+      </c>
+      <c r="O56" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="N56" t="s">
+      <c r="P56" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="B57" s="1" t="s">
+      <c r="B57" s="2"/>
+      <c r="C57" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="H57" t="b">
-        <v>1</v>
-      </c>
-      <c r="K57" t="b">
-        <v>1</v>
-      </c>
-      <c r="L57">
-        <v>1</v>
-      </c>
-      <c r="M57" s="1" t="s">
+      <c r="J57" t="b">
+        <v>1</v>
+      </c>
+      <c r="M57" t="b">
+        <v>1</v>
+      </c>
+      <c r="N57">
+        <v>1</v>
+      </c>
+      <c r="O57" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="N57" t="s">
+      <c r="P57" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="B58" s="1" t="s">
+      <c r="B58" s="2"/>
+      <c r="C58" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="H58" t="b">
-        <v>1</v>
-      </c>
-      <c r="M58" s="1" t="s">
+      <c r="J58" t="b">
+        <v>1</v>
+      </c>
+      <c r="O58" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="N58" t="s">
+      <c r="P58" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="B59" s="1" t="s">
+      <c r="B59" s="2"/>
+      <c r="C59" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="H59" t="b">
-        <v>1</v>
-      </c>
-      <c r="M59" s="1" t="s">
+      <c r="J59" t="b">
+        <v>1</v>
+      </c>
+      <c r="O59" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="N59" t="s">
+      <c r="P59" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="B60" s="1" t="s">
+      <c r="B60" s="2"/>
+      <c r="C60" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="K60" t="b">
-        <v>1</v>
-      </c>
-      <c r="L60">
-        <v>1</v>
-      </c>
-      <c r="M60" s="1" t="s">
+      <c r="M60" t="b">
+        <v>1</v>
+      </c>
+      <c r="N60">
+        <v>1</v>
+      </c>
+      <c r="O60" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="N60" t="s">
+      <c r="P60" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="B61" s="1" t="s">
+      <c r="B61" s="2"/>
+      <c r="C61" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="K61" t="b">
-        <v>1</v>
-      </c>
-      <c r="L61">
-        <v>1</v>
-      </c>
-      <c r="M61" s="1" t="s">
+      <c r="M61" t="b">
+        <v>1</v>
+      </c>
+      <c r="N61">
+        <v>1</v>
+      </c>
+      <c r="O61" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="N61" t="s">
+      <c r="P61" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="B62" s="1" t="s">
+      <c r="B62" s="2"/>
+      <c r="C62" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="K62" t="b">
-        <v>1</v>
-      </c>
-      <c r="L62">
-        <v>1</v>
-      </c>
-      <c r="M62" s="1" t="s">
+      <c r="M62" t="b">
+        <v>1</v>
+      </c>
+      <c r="N62">
+        <v>1</v>
+      </c>
+      <c r="O62" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="N62" t="s">
+      <c r="P62" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="B63" s="1" t="s">
+      <c r="B63" s="2"/>
+      <c r="C63" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="J63" t="b">
-        <v>1</v>
-      </c>
-      <c r="L63">
+      <c r="G63" t="s">
+        <v>260</v>
+      </c>
+      <c r="L63" t="b">
+        <v>1</v>
+      </c>
+      <c r="N63">
         <v>10</v>
       </c>
-      <c r="M63" s="1" t="s">
+      <c r="O63" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="N63" t="s">
+      <c r="P63" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="B64" s="1" t="s">
+      <c r="B64" s="2"/>
+      <c r="C64" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="J64" t="b">
-        <v>1</v>
-      </c>
-      <c r="L64">
+      <c r="G64" t="s">
+        <v>260</v>
+      </c>
+      <c r="L64" t="b">
+        <v>1</v>
+      </c>
+      <c r="N64">
         <v>10</v>
       </c>
-      <c r="M64" s="1" t="s">
+      <c r="O64" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="N64" t="s">
+      <c r="P64" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="B65" s="1" t="s">
+      <c r="B65" s="2"/>
+      <c r="C65" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="J65" t="b">
-        <v>1</v>
-      </c>
-      <c r="L65">
+      <c r="G65" t="s">
+        <v>259</v>
+      </c>
+      <c r="L65" t="b">
+        <v>1</v>
+      </c>
+      <c r="N65">
         <v>10</v>
       </c>
-      <c r="M65" s="1" t="s">
+      <c r="O65" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="N65" t="s">
+      <c r="P65" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="B66" s="1" t="s">
+      <c r="B66" s="2"/>
+      <c r="C66" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="J66" t="b">
-        <v>1</v>
-      </c>
-      <c r="L66">
-        <v>1</v>
-      </c>
-      <c r="M66" s="1" t="s">
+      <c r="L66" t="b">
+        <v>1</v>
+      </c>
+      <c r="N66">
+        <v>1</v>
+      </c>
+      <c r="O66" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="N66" t="s">
+      <c r="P66" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="B67" s="1" t="s">
+      <c r="B67" s="2"/>
+      <c r="C67" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="J67" t="b">
-        <v>1</v>
-      </c>
-      <c r="L67">
-        <v>1</v>
-      </c>
-      <c r="M67" s="1" t="s">
+      <c r="L67" t="b">
+        <v>1</v>
+      </c>
+      <c r="N67">
+        <v>1</v>
+      </c>
+      <c r="O67" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="N67" t="s">
+      <c r="P67" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="H68" t="b">
-        <v>1</v>
-      </c>
-      <c r="N68" t="s">
+    <row r="68" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A68" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="B68" s="2"/>
+      <c r="C68" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="J68" t="b">
+        <v>1</v>
+      </c>
+      <c r="P68" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="H69" t="b">
-        <v>1</v>
-      </c>
-      <c r="N69" t="s">
+    <row r="69" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A69" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="B69" s="2"/>
+      <c r="C69" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="J69" t="b">
+        <v>1</v>
+      </c>
+      <c r="P69" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="H70" t="b">
-        <v>1</v>
-      </c>
-      <c r="N70" t="s">
+    <row r="70" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A70" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="B70" s="2"/>
+      <c r="C70" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="J70" t="b">
+        <v>1</v>
+      </c>
+      <c r="P70" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="71" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="H71" t="b">
-        <v>1</v>
-      </c>
-      <c r="N71" t="s">
+    <row r="71" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A71" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="B71" s="2"/>
+      <c r="C71" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="J71" t="b">
+        <v>1</v>
+      </c>
+      <c r="P71" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="72" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="H72" t="b">
-        <v>1</v>
-      </c>
-      <c r="N72" t="s">
+    <row r="72" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A72" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="B72" s="2"/>
+      <c r="C72" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="J72" t="b">
+        <v>1</v>
+      </c>
+      <c r="P72" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="73" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B73" s="1" t="s">
+      <c r="B73" s="2"/>
+      <c r="C73" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="H73" t="b">
-        <v>1</v>
-      </c>
-      <c r="M73" s="1" t="s">
+      <c r="J73" t="b">
+        <v>1</v>
+      </c>
+      <c r="O73" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="N73" t="s">
+      <c r="P73" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="74" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="H74" t="b">
-        <v>1</v>
-      </c>
-      <c r="N74" t="s">
+    <row r="74" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A74" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="B74" s="2"/>
+      <c r="C74" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="J74" t="b">
+        <v>1</v>
+      </c>
+      <c r="P74" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="75" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="H75" t="b">
-        <v>1</v>
-      </c>
-      <c r="N75" t="s">
+    <row r="75" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A75" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="B75" s="2"/>
+      <c r="C75" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="J75" t="b">
+        <v>1</v>
+      </c>
+      <c r="P75" t="s">
         <v>239</v>
+      </c>
+    </row>
+    <row r="76" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A76" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="B76" s="4"/>
+      <c r="C76" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="F76" t="b">
+        <v>1</v>
+      </c>
+      <c r="G76">
+        <v>1185</v>
+      </c>
+      <c r="L76" t="b">
+        <v>1</v>
+      </c>
+      <c r="N76">
+        <v>1</v>
+      </c>
+      <c r="O76" s="1" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="77" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A77" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="B77" s="2"/>
+      <c r="C77" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="F77" t="b">
+        <v>1</v>
+      </c>
+      <c r="G77">
+        <v>110</v>
+      </c>
+      <c r="L77" t="b">
+        <v>1</v>
+      </c>
+      <c r="N77">
+        <v>1</v>
+      </c>
+      <c r="O77" t="s">
+        <v>175</v>
       </c>
     </row>
   </sheetData>

</xml_diff>